<commit_message>
Created UC 8 test methodology
</commit_message>
<xml_diff>
--- a/Análise/Test Scenarios - Vitor.xlsx
+++ b/Análise/Test Scenarios - Vitor.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="134">
   <si>
     <t>Project Name</t>
   </si>
@@ -438,9 +438,6 @@
     <t>TC_Define_006</t>
   </si>
   <si>
-    <t>Be registered as a Freelancer in the Platform</t>
-  </si>
-  <si>
     <t>Applying to Task Functionality</t>
   </si>
   <si>
@@ -450,9 +447,116 @@
     <t>Successful application. Freelancer is now one of the candidates for the task he has applied to.</t>
   </si>
   <si>
-    <t>Valid matching requirements for task
-Valid Resumed Description
-Valid Thorough Description</t>
+    <t>1. Freelancer enters valid username and password to log in
+2. Administrative verifies Freelancers competences
+3. Application submited within the timeframe set for the task
+4. Requirements for the task matchs the Freelancer competences</t>
+  </si>
+  <si>
+    <t>1. Freelancer enters invalid username and/or password to log in
+2. Administrative verifies Freelancers competences
+3. Application submited within the timeframe set for the task
+4. Requirements for the task matchs the Freelancer competences</t>
+  </si>
+  <si>
+    <t>The user should not be able to become a candidate for the task he wants to apply to.</t>
+  </si>
+  <si>
+    <t>Unsuccessful application. Freelancers must be registered in Platform to be able to apply for taks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelancer is NOT Registered/ Cannot Sign in
+Freelancer Competences are verified
+The application is within the timeframe for the task
+Requirements for task are matched
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelancer is Registered and able to sign in
+Freelancer Competences are verified
+The application is within the timeframe for the task
+Requirements for task are matched
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelancer is Registered and able to sign in
+Freelancer Competences are NOT verified
+The application is within the timeframe for the task
+Requirements for task are matched
+</t>
+  </si>
+  <si>
+    <t>1. Enters valid username and password
+2. enters valid competences wich are verified
+3. Application time: 09:00:00 on 01.01.2020 / Timeframe for application: 08:00:00 to 10:00:00 on 01.01.2020
+4. matching requirements:
+SQL -&gt; SQL
+English -&gt; English
+Proficient -&gt; Proficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enters invalid username and password
+</t>
+  </si>
+  <si>
+    <t>1. Enters valid username and password
+2. enters invalid competences wich are not approved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelancer is Registered and able to sign in
+Freelancer Competences are verified
+The application is NOT within the timeframe for the task
+Requirements for task are matched
+</t>
+  </si>
+  <si>
+    <t>1. Freelancer enters valid username and password to log in
+2. Administrative verifies Freelancers competences
+3. Application NOT submited within the timeframe set for the task
+4. Requirements for the task matchs the Freelancer competences</t>
+  </si>
+  <si>
+    <t>1. Freelancer enters valid username and password to log in
+2. Administrative does NOT approve Freelancers competences as they are untrue
+3. Application submited within the timeframe set for the task
+4. Requirements for the task matchs the Freelancer competences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Enters valid username and password
+2. enters valid competences wich are verified
+3. Application time: 11:00:00 on 01.01.2020 / Timeframe for application: 08:00:00 to 10:00:00 on 01.01.2020
+</t>
+  </si>
+  <si>
+    <t>Unsuccessful application. Freelancers must have competences validated to be able to apply for taks.</t>
+  </si>
+  <si>
+    <t>Unsuccessful application. Freelancers must apply for tasks within the timeframe set.</t>
+  </si>
+  <si>
+    <t>1. Freelancer enters valid username and password to log in
+2. Administrative verifies Freelancers competences
+3. Application submited within the timeframe set for the task
+4. Requirements for the task DO NOT match the Freelancer competences</t>
+  </si>
+  <si>
+    <t>1. Enters valid username and password
+2. enters valid competences wich are verified
+3. Application time: 09:00:00 on 01.01.2020 / Timeframe for application: 08:00:00 to 10:00:00 on 01.01.2020
+4. matching requirements:
+SQL -&gt; 
+English -&gt; English
+Proficient -&gt; Proficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freelancer is Registered and able to sign in
+Freelancer Competences are verified
+The application is within the timeframe for the task
+Requirements for task are NOT matched
+</t>
+  </si>
+  <si>
+    <t>Unsuccessful application. Freelancers competences must match the tasks requirements to be able to apply.</t>
   </si>
 </sst>
 </file>
@@ -525,7 +629,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -535,6 +639,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -911,7 +1021,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2012,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2063,24 +2173,22 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="G8" s="5"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
@@ -2088,24 +2196,22 @@
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>112</v>
-      </c>
+      <c r="B9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="5"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
@@ -2113,124 +2219,114 @@
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>110</v>
-      </c>
+      <c r="G10" s="5"/>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="B11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="5"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="B12" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="5"/>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="B13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="5"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="234" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>104</v>
-      </c>
+      <c r="B14" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="G14" s="5"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
@@ -2238,49 +2334,45 @@
       <c r="A15" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B15" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="G15" s="5"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="78" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="B16" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="5"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
@@ -2288,30 +2380,33 @@
       <c r="A17" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B17"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>40</v>
-      </c>
+      <c r="G18" s="5"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>

</xml_diff>

<commit_message>
update final remastered uc8
</commit_message>
<xml_diff>
--- a/Análise/Test Scenarios - Vitor.xlsx
+++ b/Análise/Test Scenarios - Vitor.xlsx
@@ -444,9 +444,6 @@
     <t>The user should be able to become a candidate for the task he has applied to.</t>
   </si>
   <si>
-    <t>Successful application. Freelancer is now one of the candidates for the task he has applied to.</t>
-  </si>
-  <si>
     <t>1. Freelancer enters valid username and password to log in
 2. Administrative verifies Freelancers competences
 3. Application submited within the timeframe set for the task
@@ -460,9 +457,6 @@
   </si>
   <si>
     <t>The user should not be able to become a candidate for the task he wants to apply to.</t>
-  </si>
-  <si>
-    <t>Unsuccessful application. Freelancers must be registered in Platform to be able to apply for taks.</t>
   </si>
   <si>
     <t xml:space="preserve">Freelancer is NOT Registered/ Cannot Sign in
@@ -528,12 +522,6 @@
 </t>
   </si>
   <si>
-    <t>Unsuccessful application. Freelancers must have competences validated to be able to apply for taks.</t>
-  </si>
-  <si>
-    <t>Unsuccessful application. Freelancers must apply for tasks within the timeframe set.</t>
-  </si>
-  <si>
     <t>1. Freelancer enters valid username and password to log in
 2. Administrative verifies Freelancers competences
 3. Application submited within the timeframe set for the task
@@ -556,7 +544,19 @@
 </t>
   </si>
   <si>
-    <t>Unsuccessful application. Freelancers competences must match the tasks requirements to be able to apply.</t>
+    <t>POP UP: Successful application. Freelancer is now one of the candidates for the task he has applied to.</t>
+  </si>
+  <si>
+    <t>Throws exception IllegalArgument: Unsuccessful application. Freelancers competences must match the tasks requirements to be able to apply.</t>
+  </si>
+  <si>
+    <t>Throws exception IllegalArgument: Unsuccessful application. Freelancers must apply for tasks within the timeframe set.</t>
+  </si>
+  <si>
+    <t>Throws exception IllegalArgument: Unsuccessful application. Freelancers must have competences validated to be able to apply for taks.</t>
+  </si>
+  <si>
+    <t>Throws exception IllegalArgument: Unsuccessful application. Freelancers must be registered in Platform to be able to apply for taks.</t>
   </si>
 </sst>
 </file>
@@ -2122,8 +2122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.09765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2243,19 +2243,19 @@
         <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>120</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="1"/>
@@ -2266,19 +2266,19 @@
         <v>20</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>115</v>
-      </c>
       <c r="D12" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>130</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
@@ -2312,19 +2312,19 @@
         <v>26</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="E14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>127</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>131</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="1"/>
@@ -2338,39 +2338,39 @@
         <v>112</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="78" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>117</v>
+        <v>133</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="1"/>

</xml_diff>